<commit_message>
ran experiment2. lots of plots.
</commit_message>
<xml_diff>
--- a/Summary Analysis.xlsx
+++ b/Summary Analysis.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1380" windowWidth="21620" windowHeight="14440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="820" yWindow="0" windowWidth="27900" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="time spent" sheetId="1" r:id="rId1"/>
     <sheet name="knowledge by pref" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="homogeneity" sheetId="5" r:id="rId3"/>
+    <sheet name="chanceofLearn" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
   <si>
     <t>x axis</t>
   </si>
@@ -152,15 +153,6 @@
     <t>B</t>
   </si>
   <si>
-    <t xml:space="preserve">6 2 2 2 </t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>num</t>
-  </si>
-  <si>
     <t>mean final knowledge</t>
   </si>
   <si>
@@ -216,13 +208,49 @@
   </si>
   <si>
     <t>SD Indiv</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>numA</t>
+  </si>
+  <si>
+    <t>numB</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>data from 10 repeats</t>
+  </si>
+  <si>
+    <t>DESCRIPTIVE DATA FOR A = 18, B = 2</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>When 50 lazy + 50 hardworking</t>
+  </si>
+  <si>
+    <t>When 50 hardworking</t>
+  </si>
+  <si>
+    <t>when 50 lazy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,6 +280,15 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
@@ -296,7 +333,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -316,13 +353,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -332,6 +376,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -341,9 +386,16 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -377,13 +429,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average Amount</a:t>
+              <a:t>Knowledge acquired by personality</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Learnt</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -574,11 +621,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2142344936"/>
-        <c:axId val="2113792040"/>
+        <c:axId val="-2138785864"/>
+        <c:axId val="-2136658936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2142344936"/>
+        <c:axId val="-2138785864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -607,7 +654,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113792040"/>
+        <c:crossAx val="-2136658936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -615,7 +662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113792040"/>
+        <c:axId val="-2136658936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,7 +673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142344936"/>
+        <c:crossAx val="-2138785864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -663,6 +710,389 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>Knowledge acquired by class makeup</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>All</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Table13[numA]</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>homogeneity!$C$8:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>447.235</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>416.015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>375.5200000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>374.275</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>378.275</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>338.335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>305.07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>303.695</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>303.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Lazy</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Table13[numA]</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>homogeneity!$D$8:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>359.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>315.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>277.6999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>321.4375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>313.1200000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>285.8749999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>283.3928571428566</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>286.0875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>294.7965277777774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Hardworking</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Table13[numA]</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>homogeneity!$E$8:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>456.983333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>441.15625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>417.4428571428567</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>409.4999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>443.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>417.025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>355.6499999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>369.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>363.775</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2141410392"/>
+        <c:axId val="2113012072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2141410392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>% of lazy students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2113012072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2113012072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="200.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2141410392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1050"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -675,6 +1105,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Lazy</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -691,78 +1124,318 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$C$6:$C$15</c:f>
+              <c:f>chanceofLearn!$M$5:$M$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>0.726091797416594</c:v>
+                  <c:v>0.18942746413896</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.553171327864319</c:v>
+                  <c:v>0.565229622487435</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.211689542673625</c:v>
+                  <c:v>0.788611175977931</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.848048276296347</c:v>
+                  <c:v>0.00734881891161398</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.496886389718721</c:v>
+                  <c:v>0.877964249375288</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0768000378500802</c:v>
+                  <c:v>0.256516197719665</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.767313142791123</c:v>
+                  <c:v>0.224253178115234</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32802624595067</c:v>
+                  <c:v>0.188007552064858</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.580900602070496</c:v>
+                  <c:v>0.35220383780509</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.518117192075624</c:v>
+                  <c:v>0.936604603559188</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.881853113937672</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.136487137993647</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.498947343030066</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0379975528622342</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.441230335624789</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.820620822754073</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0570460834914189</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.679188156701133</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.689299425845487</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.816455733918</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.245319135320094</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.277399381355217</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0871349151264093</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.0677749877872407</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.0391563224567201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.870100301693533</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.833232510288532</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.68020599487277</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.52286271759612</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.434373915146732</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.412262792685266</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.120870326703281</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.636138214567394</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.728528109691222</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.0161053094301211</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.817038979282432</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.868937396711472</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.619017135524266</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.447052685513621</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.195711184834545</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.59180785320403</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.175038195584749</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.450956089627748</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.736148335653916</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.120590102949423</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.994048501388476</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.140787785385</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.451565920112083</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.082364802299603</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.858687736607071</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$D$6:$D$15</c:f>
+              <c:f>chanceofLearn!$N$5:$N$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>378.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>759.0</c:v>
+                  <c:v>93.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>919.0</c:v>
+                  <c:v>197.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>692.0</c:v>
+                  <c:v>291.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>798.0</c:v>
+                  <c:v>221.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>878.0</c:v>
+                  <c:v>99.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1002.0</c:v>
+                  <c:v>232.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>963.0</c:v>
+                  <c:v>229.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>422.0</c:v>
+                  <c:v>130.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>635.0</c:v>
+                  <c:v>265.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>316.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>261.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>325.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>333.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>246.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>418.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>272.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>327.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>208.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>178.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>327.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>303.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>177.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>286.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>270.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>186.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>356.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>13.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -772,6 +1445,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Hardworking</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -788,78 +1464,318 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$C$16:$C$25</c:f>
+              <c:f>chanceofLearn!$O$5:$O$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>0.362790717900364</c:v>
+                  <c:v>0.747596773790078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.595299068466159</c:v>
+                  <c:v>0.0526679046705278</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58844836034855</c:v>
+                  <c:v>0.403219461721053</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.765973753332548</c:v>
+                  <c:v>0.569310126639185</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.782319261075324</c:v>
+                  <c:v>0.47732026374796</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.827136423582974</c:v>
+                  <c:v>0.253203398548923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.212792832038486</c:v>
+                  <c:v>0.0338228302044576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.329148403047617</c:v>
+                  <c:v>0.0404080952691151</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.847905496668968</c:v>
+                  <c:v>0.064082946071702</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.336493213157809</c:v>
+                  <c:v>0.997578928895642</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.219413218304432</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.18662126367077</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.501415450046775</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.730040908243114</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.930273216453421</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.460937777019423</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.399602075361816</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.831427573392593</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.137651265006066</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.291924767626396</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.132150497150385</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.608154185956801</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.535340634615312</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.29796350871037</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.689252206080528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.366988960815303</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.35908173357485</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.256592457798325</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.302360018292134</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.728884640288691</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.0980540202780502</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.81787815992794</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.622556135327956</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.763082633936062</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.931801566703858</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.0855550720251612</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.607334927896482</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.313290378932293</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.134288185421604</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.676232351837639</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.620205983460014</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.0101613301905111</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.95289874678812</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.035502104093779</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.629916448469125</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.444113461728453</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.343275742837889</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.128945231010142</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.263544356373753</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.338036779838648</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$D$16:$D$25</c:f>
+              <c:f>chanceofLearn!$P$5:$P$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>693.0</c:v>
+                  <c:v>328.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>761.0</c:v>
+                  <c:v>536.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1228.0</c:v>
+                  <c:v>131.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1112.0</c:v>
+                  <c:v>318.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>630.0</c:v>
+                  <c:v>420.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1398.0</c:v>
+                  <c:v>483.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1030.0</c:v>
+                  <c:v>280.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>917.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>983.0</c:v>
+                  <c:v>738.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>966.0</c:v>
+                  <c:v>398.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>528.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>599.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>233.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>455.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>556.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>679.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>317.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>387.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>540.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>344.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>570.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>341.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>370.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>520.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>469.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>427.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>307.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>352.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>344.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>309.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,11 +1790,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2105143384"/>
-        <c:axId val="-2147144808"/>
+        <c:axId val="-2140470008"/>
+        <c:axId val="-2141180520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2105143384"/>
+        <c:axId val="-2140470008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,12 +1808,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147144808"/>
+        <c:crossAx val="-2141180520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2147144808"/>
+        <c:axId val="-2141180520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +1829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105143384"/>
+        <c:crossAx val="-2140470008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -974,20 +1890,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>425450</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1013,11 +1964,27 @@
     <tableColumn id="6" name="Prefs"/>
     <tableColumn id="2" name="A pref"/>
     <tableColumn id="3" name="Mean Knowledge"/>
-    <tableColumn id="7" name="95% CI" dataDxfId="0">
+    <tableColumn id="7" name="95% CI" dataDxfId="2">
       <calculatedColumnFormula>2*Table1[[#This Row],[SD group Knowledge]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="SD group Knowledge"/>
     <tableColumn id="8" name="SD Indiv"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A7:E16" totalsRowShown="0">
+  <autoFilter ref="A7:E16"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="numA"/>
+    <tableColumn id="6" name="numB"/>
+    <tableColumn id="3" name="Overall" dataDxfId="0"/>
+    <tableColumn id="7" name="A" dataDxfId="1">
+      <calculatedColumnFormula>2*Table13[[#This Row],[B]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="B"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1730,7 +2697,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1748,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1756,7 +2723,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -1781,40 +2748,40 @@
     </row>
     <row r="4" spans="1:20">
       <c r="H4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
         <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L4" t="s">
         <v>38</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N4" t="s">
         <v>38</v>
       </c>
       <c r="O4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="P4" t="s">
         <v>38</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="R4" t="s">
         <v>38</v>
       </c>
       <c r="S4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="T4" t="s">
         <v>38</v>
@@ -1828,7 +2795,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1913,25 +2880,25 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -1981,7 +2948,7 @@
         <v>6222</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8">
         <v>274.02</v>
@@ -2044,7 +3011,7 @@
         <v>6141</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>140.6</v>
@@ -2107,7 +3074,7 @@
         <v>6114</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D10">
         <v>352</v>
@@ -2170,7 +3137,7 @@
         <v>3333</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D11">
         <v>448</v>
@@ -2233,7 +3200,7 @@
         <v>3252</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D12">
         <v>353.1</v>
@@ -2296,7 +3263,7 @@
         <v>3225</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13">
         <v>480.2</v>
@@ -2804,7 +3771,7 @@
     </row>
     <row r="26" spans="8:20">
       <c r="H26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I26">
         <f xml:space="preserve"> AVERAGE(I5:I24)</f>
@@ -2857,7 +3824,7 @@
     </row>
     <row r="27" spans="8:20">
       <c r="H27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I27">
         <f>STDEV(I5:I24)</f>
@@ -2886,7 +3853,7 @@
     </row>
     <row r="28" spans="8:20">
       <c r="H28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I28">
         <f>I27/SQRT(20)</f>
@@ -2915,7 +3882,7 @@
     </row>
     <row r="29" spans="8:20">
       <c r="H29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I29">
         <f>2*I28</f>
@@ -2959,484 +3926,1313 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D45"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.5" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="I3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="H4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>413.6</v>
+      </c>
+      <c r="J5">
+        <v>195.10277993109699</v>
+      </c>
+      <c r="K5">
+        <v>240.5</v>
+      </c>
+      <c r="L5">
+        <v>340.11836175072898</v>
+      </c>
+      <c r="M5">
+        <v>432.83333333333297</v>
+      </c>
+      <c r="N5">
+        <v>178.38664220632401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="H6" s="7">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>431.7</v>
+      </c>
+      <c r="J6">
+        <v>243.69029093243901</v>
+      </c>
+      <c r="K6">
+        <v>571.5</v>
+      </c>
+      <c r="L6">
+        <v>391.03004999616002</v>
+      </c>
+      <c r="M6">
+        <v>416.166666666666</v>
+      </c>
+      <c r="N6">
+        <v>234.14154844000299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>367.75</v>
+      </c>
+      <c r="J7">
+        <v>174.18135588185601</v>
+      </c>
+      <c r="K7">
+        <v>419</v>
+      </c>
+      <c r="L7">
+        <v>128.69343417595101</v>
+      </c>
+      <c r="M7">
+        <v>362.05555555555497</v>
+      </c>
+      <c r="N7">
+        <v>180.52944104762301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5">
+        <v>447.23500000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <v>359.5</v>
+      </c>
+      <c r="E8">
+        <v>456.98333333333301</v>
+      </c>
+      <c r="H8" s="7">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>430.95</v>
+      </c>
+      <c r="J8">
+        <v>231.47342123198899</v>
+      </c>
+      <c r="K8">
+        <v>369</v>
+      </c>
+      <c r="L8">
+        <v>195.16147160748699</v>
+      </c>
+      <c r="M8">
+        <v>437.83333333333297</v>
+      </c>
+      <c r="N8">
+        <v>239.04251406269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5">
+        <v>416.01499999999999</v>
+      </c>
+      <c r="D9" s="5">
+        <v>315.45</v>
+      </c>
+      <c r="E9">
+        <v>441.15625</v>
+      </c>
+      <c r="H9" s="7">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>454.95</v>
+      </c>
+      <c r="J9">
+        <v>132.782162324534</v>
+      </c>
+      <c r="K9">
+        <v>340</v>
+      </c>
+      <c r="L9">
+        <v>28.284271247461898</v>
+      </c>
+      <c r="M9">
+        <v>467.722222222222</v>
+      </c>
+      <c r="N9">
+        <v>133.90681815244599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5">
+        <v>375.5200000000001</v>
+      </c>
+      <c r="D10" s="5">
+        <v>277.69999999999948</v>
+      </c>
+      <c r="E10">
+        <v>417.44285714285672</v>
+      </c>
+      <c r="H10" s="7">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>475</v>
+      </c>
+      <c r="J10">
+        <v>199.06677007318001</v>
+      </c>
+      <c r="K10">
+        <v>225.5</v>
+      </c>
+      <c r="L10">
+        <v>304.763022691402</v>
+      </c>
+      <c r="M10">
+        <v>502.722222222222</v>
+      </c>
+      <c r="N10">
+        <v>175.18219274114199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5">
+        <v>374.27499999999998</v>
+      </c>
+      <c r="D11" s="5">
+        <v>321.4375</v>
+      </c>
+      <c r="E11">
+        <v>409.49999999999955</v>
+      </c>
+      <c r="H11" s="7">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>497.5</v>
+      </c>
+      <c r="J11">
+        <v>163.892294542868</v>
+      </c>
+      <c r="K11">
+        <v>438.5</v>
+      </c>
+      <c r="L11">
+        <v>98.287842584930104</v>
+      </c>
+      <c r="M11">
+        <v>504.05555555555497</v>
+      </c>
+      <c r="N11">
+        <v>170.28642729313799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5">
+        <v>378.27499999999998</v>
+      </c>
+      <c r="D12" s="5">
+        <v>313.12000000000006</v>
+      </c>
+      <c r="E12">
+        <v>443.43</v>
+      </c>
+      <c r="H12" s="7">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>510.65</v>
+      </c>
+      <c r="J12">
+        <v>177.585050046449</v>
+      </c>
+      <c r="K12">
+        <v>381.5</v>
+      </c>
+      <c r="L12">
+        <v>24.7487373415291</v>
+      </c>
+      <c r="M12">
+        <v>525</v>
+      </c>
+      <c r="N12">
+        <v>181.74222210074799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>338.33499999999998</v>
+      </c>
+      <c r="D13" s="5">
+        <v>285.8749999999996</v>
+      </c>
+      <c r="E13">
+        <v>417.02499999999998</v>
+      </c>
+      <c r="H13" s="7">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>415.65</v>
+      </c>
+      <c r="J13">
+        <v>192.31998418206399</v>
+      </c>
+      <c r="K13">
+        <v>235</v>
+      </c>
+      <c r="L13">
+        <v>67.882250993908499</v>
+      </c>
+      <c r="M13">
+        <v>435.722222222222</v>
+      </c>
+      <c r="N13">
+        <v>191.836880940263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6">
+        <v>305.07</v>
+      </c>
+      <c r="D14" s="6">
+        <v>283.3928571428566</v>
+      </c>
+      <c r="E14" s="4">
+        <v>355.64999999999975</v>
+      </c>
+      <c r="H14" s="7">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>474.6</v>
+      </c>
+      <c r="J14">
+        <v>163.92565709074199</v>
+      </c>
+      <c r="K14">
+        <v>374.5</v>
+      </c>
+      <c r="L14">
+        <v>153.44217151748001</v>
+      </c>
+      <c r="M14">
+        <v>485.722222222222</v>
+      </c>
+      <c r="N14">
+        <v>165.34271202052</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>80</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>303.69500000000005</v>
+      </c>
+      <c r="D15" s="5">
+        <v>286.08749999999998</v>
+      </c>
+      <c r="E15">
+        <v>369.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>90</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>303.05</v>
+      </c>
+      <c r="D16" s="5">
+        <v>294.79652777777738</v>
+      </c>
+      <c r="E16">
+        <v>363.77499999999998</v>
+      </c>
+      <c r="H16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16">
+        <f xml:space="preserve"> AVERAGE(I5:I14)</f>
+        <v>447.23500000000001</v>
+      </c>
+      <c r="J16">
+        <f>AVERAGE(J5:J14)</f>
+        <v>187.40197662372185</v>
+      </c>
+      <c r="K16">
+        <f xml:space="preserve"> AVERAGE(K5:K14)</f>
+        <v>359.5</v>
+      </c>
+      <c r="L16">
+        <f>AVERAGE(L5:L14)</f>
+        <v>173.24116139070384</v>
+      </c>
+      <c r="M16">
+        <f xml:space="preserve"> AVERAGE(M5:M14)</f>
+        <v>456.98333333333301</v>
+      </c>
+      <c r="N16">
+        <f>AVERAGE(N5:N14)</f>
+        <v>185.03973990048968</v>
+      </c>
+    </row>
+    <row r="17" spans="4:13">
+      <c r="D17" s="3"/>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17">
+        <f>STDEV(I5:I14)</f>
+        <v>43.564282324450666</v>
+      </c>
+      <c r="K17">
+        <f>STDEV(L5:L14)</f>
+        <v>131.32487282393305</v>
+      </c>
+      <c r="M17">
+        <f>STDEV(N5:N14)</f>
+        <v>31.209593497253099</v>
+      </c>
+    </row>
+    <row r="18" spans="4:13">
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18">
+        <f>I17/SQRT(20)</f>
+        <v>9.7412696668464225</v>
+      </c>
+      <c r="K18">
+        <f>K17/SQRT(20)</f>
+        <v>29.365134277082905</v>
+      </c>
+      <c r="M18">
+        <f>M17/SQRT(20)</f>
+        <v>6.9786772609993326</v>
+      </c>
+    </row>
+    <row r="19" spans="4:13">
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19">
+        <f>2*I18</f>
+        <v>19.482539333692845</v>
+      </c>
+      <c r="K19">
+        <f>2*K18</f>
+        <v>58.730268554165811</v>
+      </c>
+      <c r="M19">
+        <f>2*M18</f>
+        <v>13.957354521998665</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="M1:U54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="2" spans="1:4">
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="1" spans="13:21">
+      <c r="M1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="13:21">
+      <c r="M2">
+        <v>6222</v>
+      </c>
+      <c r="O2">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="3" spans="13:21">
+      <c r="M3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="O3" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="4" spans="13:21">
+      <c r="M4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="13:21">
+      <c r="M5">
+        <v>0.18942746413896</v>
+      </c>
+      <c r="N5">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6">
-        <v>0.72609179741659402</v>
-      </c>
-      <c r="D6">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7">
-        <v>0.553171327864319</v>
-      </c>
-      <c r="D7">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8">
-        <v>0.211689542673625</v>
-      </c>
-      <c r="D8">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9">
-        <v>0.84804827629634705</v>
-      </c>
-      <c r="D9">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10">
-        <v>0.49688638971872101</v>
-      </c>
-      <c r="D10">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11">
-        <v>7.6800037850080202E-2</v>
-      </c>
-      <c r="D11">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12">
-        <v>0.76731314279112295</v>
-      </c>
-      <c r="D12">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13">
-        <v>0.32802624595066998</v>
-      </c>
-      <c r="D13">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14">
-        <v>0.58090060207049599</v>
-      </c>
-      <c r="D14">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15">
-        <v>0.51811719207562401</v>
-      </c>
-      <c r="D15">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16">
-        <v>0.36279071790036399</v>
-      </c>
-      <c r="D16">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17">
-        <v>0.59529906846615899</v>
-      </c>
-      <c r="D17">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18">
-        <v>0.58844836034854997</v>
-      </c>
-      <c r="D18">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19">
-        <v>0.76597375333254802</v>
-      </c>
-      <c r="D19">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20">
-        <v>0.78231926107532401</v>
-      </c>
-      <c r="D20">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21">
-        <v>0.82713642358297401</v>
-      </c>
-      <c r="D21">
-        <v>1398</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22">
-        <v>0.21279283203848601</v>
-      </c>
-      <c r="D22">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23">
-        <v>0.329148403047617</v>
-      </c>
-      <c r="D23">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24">
-        <v>0.84790549666896797</v>
-      </c>
-      <c r="D24">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25">
-        <v>0.336493213157809</v>
-      </c>
-      <c r="D25">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
+      <c r="O5">
+        <v>0.74759677379007805</v>
+      </c>
+      <c r="P5">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="6" spans="13:21">
+      <c r="M6">
+        <v>0.56522962248743502</v>
+      </c>
+      <c r="N6">
+        <v>93</v>
+      </c>
+      <c r="O6">
+        <v>5.2667904670527801E-2</v>
+      </c>
+      <c r="P6">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="7" spans="13:21">
+      <c r="M7">
+        <v>0.78861117597793096</v>
+      </c>
+      <c r="N7">
+        <v>197</v>
+      </c>
+      <c r="O7">
+        <v>0.403219461721053</v>
+      </c>
+      <c r="P7">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="13:21">
+      <c r="M8">
+        <v>7.3488189116139796E-3</v>
+      </c>
+      <c r="N8">
+        <v>291</v>
+      </c>
+      <c r="O8">
+        <v>0.56931012663918501</v>
+      </c>
+      <c r="P8">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="13:21">
+      <c r="M9">
+        <v>0.87796424937528805</v>
+      </c>
+      <c r="N9">
+        <v>221</v>
+      </c>
+      <c r="O9">
+        <v>0.47732026374795999</v>
+      </c>
+      <c r="P9">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10" spans="13:21">
+      <c r="M10">
+        <v>0.256516197719665</v>
+      </c>
+      <c r="N10">
+        <v>99</v>
+      </c>
+      <c r="O10">
+        <v>0.25320339854892299</v>
+      </c>
+      <c r="P10">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="11" spans="13:21">
+      <c r="M11">
+        <v>0.22425317811523399</v>
+      </c>
+      <c r="N11">
+        <v>232</v>
+      </c>
+      <c r="O11">
+        <v>3.3822830204457602E-2</v>
+      </c>
+      <c r="P11">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="13:21">
+      <c r="M12">
+        <v>0.188007552064858</v>
+      </c>
+      <c r="N12">
+        <v>229</v>
+      </c>
+      <c r="O12">
+        <v>4.0408095269115103E-2</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="13:21">
+      <c r="M13">
+        <v>0.35220383780509001</v>
+      </c>
+      <c r="N13">
+        <v>130</v>
+      </c>
+      <c r="O13">
+        <v>6.4082946071701993E-2</v>
+      </c>
+      <c r="P13">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="14" spans="13:21">
+      <c r="M14">
+        <v>0.93660460355918795</v>
+      </c>
+      <c r="N14">
+        <v>265</v>
+      </c>
+      <c r="O14">
+        <v>0.99757892889564204</v>
+      </c>
+      <c r="P14">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="15" spans="13:21">
+      <c r="M15">
+        <v>0.88185311393767196</v>
+      </c>
+      <c r="N15">
+        <v>316</v>
+      </c>
+      <c r="O15">
+        <v>0.219413218304432</v>
+      </c>
+      <c r="P15">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="16" spans="13:21">
+      <c r="M16">
+        <v>0.13648713799364701</v>
+      </c>
+      <c r="N16">
+        <v>28</v>
+      </c>
+      <c r="O16">
+        <v>0.18662126367077</v>
+      </c>
+      <c r="P16">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="17" spans="13:16">
+      <c r="M17">
+        <v>0.49894734303006599</v>
+      </c>
+      <c r="N17">
+        <v>180</v>
+      </c>
+      <c r="O17">
+        <v>0.50141545004677501</v>
+      </c>
+      <c r="P17">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="18" spans="13:16">
+      <c r="M18">
+        <v>3.7997552862234198E-2</v>
+      </c>
+      <c r="N18">
+        <v>261</v>
+      </c>
+      <c r="O18">
+        <v>0.73004090824311396</v>
+      </c>
+      <c r="P18">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="13:16">
+      <c r="M19">
+        <v>0.44123033562478903</v>
+      </c>
+      <c r="N19">
+        <v>325</v>
+      </c>
+      <c r="O19">
+        <v>0.93027321645342098</v>
+      </c>
+      <c r="P19">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="20" spans="13:16">
+      <c r="M20">
+        <v>0.820620822754073</v>
+      </c>
+      <c r="N20">
+        <v>140</v>
+      </c>
+      <c r="O20">
+        <v>0.46093777701942301</v>
+      </c>
+      <c r="P20">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="21" spans="13:16">
+      <c r="M21">
+        <v>5.7046083491418903E-2</v>
+      </c>
+      <c r="N21">
+        <v>333</v>
+      </c>
+      <c r="O21">
+        <v>0.39960207536181602</v>
+      </c>
+      <c r="P21">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="13:16">
+      <c r="M22">
+        <v>0.67918815670113297</v>
+      </c>
+      <c r="N22">
+        <v>152</v>
+      </c>
+      <c r="O22">
+        <v>0.83142757339259299</v>
+      </c>
+      <c r="P22">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="13:16">
+      <c r="M23">
+        <v>0.68929942584548698</v>
+      </c>
+      <c r="N23">
+        <v>310</v>
+      </c>
+      <c r="O23">
+        <v>0.137651265006066</v>
+      </c>
+      <c r="P23">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="13:16">
+      <c r="M24">
+        <v>0.81645573391799997</v>
+      </c>
+      <c r="N24">
+        <v>68</v>
+      </c>
+      <c r="O24">
+        <v>0.29192476762639602</v>
+      </c>
+      <c r="P24">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="25" spans="13:16">
+      <c r="M25">
+        <v>0.245319135320094</v>
+      </c>
+      <c r="N25">
+        <v>246</v>
+      </c>
+      <c r="O25">
+        <v>0.13215049715038499</v>
+      </c>
+      <c r="P25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="13:16">
+      <c r="M26">
+        <v>0.27739938135521702</v>
+      </c>
+      <c r="N26">
+        <v>418</v>
+      </c>
+      <c r="O26">
+        <v>0.60815418595680104</v>
+      </c>
+      <c r="P26">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32">
-        <v>2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
-        <v>2</v>
-      </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35">
-        <v>2</v>
-      </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36">
-        <v>2</v>
-      </c>
-      <c r="B36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37">
-        <v>2</v>
-      </c>
-      <c r="B37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38">
-        <v>2</v>
-      </c>
-      <c r="B38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40">
-        <v>2</v>
-      </c>
-      <c r="B40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42">
-        <v>2</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43">
-        <v>2</v>
-      </c>
-      <c r="B43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44">
-        <v>2</v>
-      </c>
-      <c r="B44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45">
-        <v>2</v>
-      </c>
-      <c r="B45" t="s">
-        <v>42</v>
+    </row>
+    <row r="27" spans="13:16">
+      <c r="M27">
+        <v>8.7134915126409307E-2</v>
+      </c>
+      <c r="N27">
+        <v>20</v>
+      </c>
+      <c r="O27">
+        <v>0.53534063461531201</v>
+      </c>
+      <c r="P27">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="13:16">
+      <c r="M28">
+        <v>6.7774987787240698E-2</v>
+      </c>
+      <c r="N28">
+        <v>272</v>
+      </c>
+      <c r="O28">
+        <v>0.29796350871036997</v>
+      </c>
+      <c r="P28">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="29" spans="13:16">
+      <c r="M29">
+        <v>3.91563224567201E-2</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29">
+        <v>0.68925220608052795</v>
+      </c>
+      <c r="P29">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="13:16">
+      <c r="M30">
+        <v>0.87010030169353303</v>
+      </c>
+      <c r="N30">
+        <v>327</v>
+      </c>
+      <c r="O30">
+        <v>0.36698896081530302</v>
+      </c>
+      <c r="P30">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="13:16">
+      <c r="M31">
+        <v>0.83323251028853196</v>
+      </c>
+      <c r="N31">
+        <v>208</v>
+      </c>
+      <c r="O31">
+        <v>0.35908173357485001</v>
+      </c>
+      <c r="P31">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="13:16">
+      <c r="M32">
+        <v>0.68020599487277</v>
+      </c>
+      <c r="N32">
+        <v>147</v>
+      </c>
+      <c r="O32">
+        <v>0.25659245779832501</v>
+      </c>
+      <c r="P32">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="13:16">
+      <c r="M33">
+        <v>0.52286271759612002</v>
+      </c>
+      <c r="N33">
+        <v>117</v>
+      </c>
+      <c r="O33">
+        <v>0.30236001829213399</v>
+      </c>
+      <c r="P33">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="34" spans="13:16">
+      <c r="M34">
+        <v>0.43437391514673201</v>
+      </c>
+      <c r="N34">
+        <v>65</v>
+      </c>
+      <c r="O34">
+        <v>0.72888464028869104</v>
+      </c>
+      <c r="P34">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="13:16">
+      <c r="M35">
+        <v>0.412262792685266</v>
+      </c>
+      <c r="N35">
+        <v>173</v>
+      </c>
+      <c r="O35">
+        <v>9.80540202780502E-2</v>
+      </c>
+      <c r="P35">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="36" spans="13:16">
+      <c r="M36">
+        <v>0.120870326703281</v>
+      </c>
+      <c r="N36">
+        <v>23</v>
+      </c>
+      <c r="O36">
+        <v>0.81787815992794</v>
+      </c>
+      <c r="P36">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="13:16">
+      <c r="M37">
+        <v>0.63613821456739394</v>
+      </c>
+      <c r="N37">
+        <v>178</v>
+      </c>
+      <c r="O37">
+        <v>0.62255613532795595</v>
+      </c>
+      <c r="P37">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="38" spans="13:16">
+      <c r="M38">
+        <v>0.72852810969122195</v>
+      </c>
+      <c r="N38">
+        <v>327</v>
+      </c>
+      <c r="O38">
+        <v>0.76308263393606202</v>
+      </c>
+      <c r="P38">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="39" spans="13:16">
+      <c r="M39">
+        <v>1.61053094301211E-2</v>
+      </c>
+      <c r="N39">
+        <v>260</v>
+      </c>
+      <c r="O39">
+        <v>0.93180156670385805</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="13:16">
+      <c r="M40">
+        <v>0.81703897928243197</v>
+      </c>
+      <c r="N40">
+        <v>78</v>
+      </c>
+      <c r="O40">
+        <v>8.5555072025161202E-2</v>
+      </c>
+      <c r="P40">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="41" spans="13:16">
+      <c r="M41">
+        <v>0.86893739671147197</v>
+      </c>
+      <c r="N41">
+        <v>280</v>
+      </c>
+      <c r="O41">
+        <v>0.60733492789648202</v>
+      </c>
+      <c r="P41">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="42" spans="13:16">
+      <c r="M42">
+        <v>0.61901713552426596</v>
+      </c>
+      <c r="N42">
+        <v>303</v>
+      </c>
+      <c r="O42">
+        <v>0.313290378932293</v>
+      </c>
+      <c r="P42">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="13:16">
+      <c r="M43">
+        <v>0.44705268551362098</v>
+      </c>
+      <c r="N43">
+        <v>177</v>
+      </c>
+      <c r="O43">
+        <v>0.13428818542160401</v>
+      </c>
+      <c r="P43">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="13:16">
+      <c r="M44">
+        <v>0.195711184834545</v>
+      </c>
+      <c r="N44">
+        <v>165</v>
+      </c>
+      <c r="O44">
+        <v>0.67623235183763897</v>
+      </c>
+      <c r="P44">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="45" spans="13:16">
+      <c r="M45">
+        <v>0.59180785320402995</v>
+      </c>
+      <c r="N45">
+        <v>120</v>
+      </c>
+      <c r="O45">
+        <v>0.62020598346001399</v>
+      </c>
+      <c r="P45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="13:16">
+      <c r="M46">
+        <v>0.17503819558474901</v>
+      </c>
+      <c r="N46">
+        <v>286</v>
+      </c>
+      <c r="O46">
+        <v>1.01613301905111E-2</v>
+      </c>
+      <c r="P46">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="47" spans="13:16">
+      <c r="M47">
+        <v>0.45095608962774802</v>
+      </c>
+      <c r="N47">
+        <v>270</v>
+      </c>
+      <c r="O47">
+        <v>0.95289874678812003</v>
+      </c>
+      <c r="P47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="13:16">
+      <c r="M48">
+        <v>0.73614833565391602</v>
+      </c>
+      <c r="N48">
+        <v>440</v>
+      </c>
+      <c r="O48">
+        <v>3.5502104093778998E-2</v>
+      </c>
+      <c r="P48">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="49" spans="13:16">
+      <c r="M49">
+        <v>0.120590102949423</v>
+      </c>
+      <c r="N49">
+        <v>96</v>
+      </c>
+      <c r="O49">
+        <v>0.62991644846912498</v>
+      </c>
+      <c r="P49">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="50" spans="13:16">
+      <c r="M50">
+        <v>0.994048501388476</v>
+      </c>
+      <c r="N50">
+        <v>33</v>
+      </c>
+      <c r="O50">
+        <v>0.44411346172845301</v>
+      </c>
+      <c r="P50">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="51" spans="13:16">
+      <c r="M51">
+        <v>0.140787785385</v>
+      </c>
+      <c r="N51">
+        <v>186</v>
+      </c>
+      <c r="O51">
+        <v>0.34327574283788898</v>
+      </c>
+      <c r="P51">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="52" spans="13:16">
+      <c r="M52">
+        <v>0.45156592011208302</v>
+      </c>
+      <c r="N52">
+        <v>356</v>
+      </c>
+      <c r="O52">
+        <v>0.12894523101014199</v>
+      </c>
+      <c r="P52">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="53" spans="13:16">
+      <c r="M53">
+        <v>8.2364802299602996E-2</v>
+      </c>
+      <c r="N53">
+        <v>110</v>
+      </c>
+      <c r="O53">
+        <v>0.26354435637375301</v>
+      </c>
+      <c r="P53">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="54" spans="13:16">
+      <c r="M54">
+        <v>0.85868773660707098</v>
+      </c>
+      <c r="N54">
+        <v>13</v>
+      </c>
+      <c r="O54">
+        <v>0.33803677983864799</v>
+      </c>
+      <c r="P54">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trial data for chanceQN
</commit_message>
<xml_diff>
--- a/Summary Analysis.xlsx
+++ b/Summary Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="0" windowWidth="27900" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="820" yWindow="0" windowWidth="27900" windowHeight="17560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="time spent" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
   <si>
     <t>x axis</t>
   </si>
@@ -243,7 +243,13 @@
     <t>When 50 hardworking</t>
   </si>
   <si>
-    <t>when 50 lazy</t>
+    <t>chance of learn</t>
+  </si>
+  <si>
+    <t>knowledge</t>
+  </si>
+  <si>
+    <t>chance of question</t>
   </si>
 </sst>
 </file>
@@ -333,8 +339,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -366,7 +386,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -377,6 +397,13 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -387,6 +414,13 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -621,11 +655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2138785864"/>
-        <c:axId val="-2136658936"/>
+        <c:axId val="2074555416"/>
+        <c:axId val="2075838776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2138785864"/>
+        <c:axId val="2074555416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136658936"/>
+        <c:crossAx val="2075838776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -662,7 +696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136658936"/>
+        <c:axId val="2075838776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,7 +707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138785864"/>
+        <c:crossAx val="2074555416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -984,11 +1018,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2141410392"/>
-        <c:axId val="2113012072"/>
+        <c:axId val="2075905640"/>
+        <c:axId val="2075911096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2141410392"/>
+        <c:axId val="2075905640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1051,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113012072"/>
+        <c:crossAx val="2075911096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1025,7 +1059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113012072"/>
+        <c:axId val="2075911096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200.0"/>
@@ -1036,7 +1070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141410392"/>
+        <c:crossAx val="2075905640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1790,11 +1824,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140470008"/>
-        <c:axId val="-2141180520"/>
+        <c:axId val="2075924536"/>
+        <c:axId val="2075929624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140470008"/>
+        <c:axId val="2075924536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,12 +1842,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141180520"/>
+        <c:crossAx val="2075929624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2141180520"/>
+        <c:axId val="2075929624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1829,7 +1863,818 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140470008"/>
+        <c:crossAx val="2075924536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>chanceofLearn!$T$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>chance of question</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.241935570491001"/>
+                  <c:y val="-0.107003881107154"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>chanceofLearn!$S$5:$S$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>413.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>298.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>424.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>177.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>437.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>184.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>119.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>243.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>486.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>268.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>232.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>218.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>294.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>195.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>273.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>267.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>109.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>99.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>343.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>201.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>352.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>318.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>105.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>183.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>189.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>275.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>327.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>401.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>274.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>111.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>198.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>199.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>313.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>241.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>174.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>chanceofLearn!$T$5:$T$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.0101681687581994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.924059187398965</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.671923080582398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.300345038791278</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.887049547760183</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93434621524268</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8617414744101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.314129998318602</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.421466794876079</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.279896678709179</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22490658331731</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.847809132411297</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.271025855185944</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.243228579855159</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.137403131872585</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.989531248923586</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.683504543406658</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.398867870126624</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.386523487152956</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.828222361436053</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.570882246041371</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.698379666744779</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.484558047313068</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.0443367678569737</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.273184963175794</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.496594538190058</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0163097436370064</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.264876206946412</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.922542402012648</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.274519344029507</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.170528142774632</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.312253362049068</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.118424292774472</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.613172519784567</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.938350326390074</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.701377740216406</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.966037805990744</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.595390948695112</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.273014483581248</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.334082834972332</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.871007598905943</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.247307847351352</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.68305595362589</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.687204610280888</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.0556982558475774</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.174271438687218</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.244354087953711</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.488985436599514</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.294797196686158</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.581468808383365</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>chanceofLearn!$U$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>chance of learn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.158997148927096"/>
+                  <c:y val="0.0807522639791729"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>chanceofLearn!$S$5:$S$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>413.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>298.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>424.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>177.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>437.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>184.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>119.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>243.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>486.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>268.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>232.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>218.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>294.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>195.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>273.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>267.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>109.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>99.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>343.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>201.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>352.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>318.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>105.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>183.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>189.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>275.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>327.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>401.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>274.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>111.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>198.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>199.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>313.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>241.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>174.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>chanceofLearn!$U$5:$U$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.519114787476908</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.751809823980001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.731187111226857</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.161970511127071</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.456925428405455</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.712695298887079</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.594288222467591</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.555520174880004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.992045678439308</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.830316605413515</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.210072827665287</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.868944822022948</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.858771883906343</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.862983925857564</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0905826176229296</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.770716750564415</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.279667067727149</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.526589601027318</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.425462040665956</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.406584559541227</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0942758971454009</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.643956968131031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.826316663453037</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.7623904321179</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.0422443356945213</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.530613102858702</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.954048463193816</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.147316949878849</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.131359564981958</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.170301287144583</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.872263152724459</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.96000903983284</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.603211931370809</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.668163141647761</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.0628679794743262</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.248615139348011</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.293694941582472</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.0739330058734623</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.618727018703072</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.913564604098959</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.447095306186328</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.555884141012396</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.472135026989178</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.701869047314147</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.755462750830933</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.488759050348489</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.562281674956691</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.0546307757634721</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.927183414621778</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.810088336564732</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2104243128"/>
+        <c:axId val="2099418648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2104243128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2099418648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2099418648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2104243128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1953,6 +2798,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1980,8 +2855,8 @@
   <tableColumns count="5">
     <tableColumn id="1" name="numA"/>
     <tableColumn id="6" name="numB"/>
-    <tableColumn id="3" name="Overall" dataDxfId="0"/>
-    <tableColumn id="7" name="A" dataDxfId="1">
+    <tableColumn id="3" name="Overall" dataDxfId="1"/>
+    <tableColumn id="7" name="A" dataDxfId="0">
       <calculatedColumnFormula>2*Table13[[#This Row],[B]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="B"/>
@@ -2696,7 +3571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -4488,8 +5363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="M1:U54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4501,9 +5376,7 @@
       <c r="R1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="U1" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="U1" s="7"/>
     </row>
     <row r="2" spans="13:21">
       <c r="M2">
@@ -4534,6 +5407,15 @@
       <c r="P4" t="s">
         <v>70</v>
       </c>
+      <c r="S4" t="s">
+        <v>74</v>
+      </c>
+      <c r="T4" t="s">
+        <v>75</v>
+      </c>
+      <c r="U4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" spans="13:21">
       <c r="M5">
@@ -4548,6 +5430,15 @@
       <c r="P5">
         <v>328</v>
       </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1.0168168758199401E-2</v>
+      </c>
+      <c r="U5">
+        <v>0.51911478747690798</v>
+      </c>
     </row>
     <row r="6" spans="13:21">
       <c r="M6">
@@ -4562,6 +5453,15 @@
       <c r="P6">
         <v>536</v>
       </c>
+      <c r="S6">
+        <v>207</v>
+      </c>
+      <c r="T6">
+        <v>0.92405918739896498</v>
+      </c>
+      <c r="U6">
+        <v>0.75180982398000096</v>
+      </c>
     </row>
     <row r="7" spans="13:21">
       <c r="M7">
@@ -4576,6 +5476,15 @@
       <c r="P7">
         <v>131</v>
       </c>
+      <c r="S7">
+        <v>413</v>
+      </c>
+      <c r="T7">
+        <v>0.67192308058239802</v>
+      </c>
+      <c r="U7">
+        <v>0.73118711122685698</v>
+      </c>
     </row>
     <row r="8" spans="13:21">
       <c r="M8">
@@ -4590,6 +5499,15 @@
       <c r="P8">
         <v>318</v>
       </c>
+      <c r="S8">
+        <v>298</v>
+      </c>
+      <c r="T8">
+        <v>0.300345038791278</v>
+      </c>
+      <c r="U8">
+        <v>0.161970511127071</v>
+      </c>
     </row>
     <row r="9" spans="13:21">
       <c r="M9">
@@ -4604,6 +5522,15 @@
       <c r="P9">
         <v>420</v>
       </c>
+      <c r="S9">
+        <v>424</v>
+      </c>
+      <c r="T9">
+        <v>0.88704954776018297</v>
+      </c>
+      <c r="U9">
+        <v>0.45692542840545503</v>
+      </c>
     </row>
     <row r="10" spans="13:21">
       <c r="M10">
@@ -4618,6 +5545,15 @@
       <c r="P10">
         <v>483</v>
       </c>
+      <c r="S10">
+        <v>177</v>
+      </c>
+      <c r="T10">
+        <v>0.93434621524268002</v>
+      </c>
+      <c r="U10">
+        <v>0.71269529888707905</v>
+      </c>
     </row>
     <row r="11" spans="13:21">
       <c r="M11">
@@ -4632,6 +5568,15 @@
       <c r="P11">
         <v>280</v>
       </c>
+      <c r="S11">
+        <v>290</v>
+      </c>
+      <c r="T11">
+        <v>0.86174147441009996</v>
+      </c>
+      <c r="U11">
+        <v>0.59428822246759105</v>
+      </c>
     </row>
     <row r="12" spans="13:21">
       <c r="M12">
@@ -4646,6 +5591,15 @@
       <c r="P12">
         <v>0</v>
       </c>
+      <c r="S12">
+        <v>437</v>
+      </c>
+      <c r="T12">
+        <v>0.314129998318602</v>
+      </c>
+      <c r="U12">
+        <v>0.55552017488000405</v>
+      </c>
     </row>
     <row r="13" spans="13:21">
       <c r="M13">
@@ -4660,6 +5614,15 @@
       <c r="P13">
         <v>738</v>
       </c>
+      <c r="S13">
+        <v>184</v>
+      </c>
+      <c r="T13">
+        <v>0.42146679487607902</v>
+      </c>
+      <c r="U13">
+        <v>0.99204567843930802</v>
+      </c>
     </row>
     <row r="14" spans="13:21">
       <c r="M14">
@@ -4674,6 +5637,15 @@
       <c r="P14">
         <v>398</v>
       </c>
+      <c r="S14">
+        <v>119</v>
+      </c>
+      <c r="T14">
+        <v>0.279896678709179</v>
+      </c>
+      <c r="U14">
+        <v>0.83031660541351504</v>
+      </c>
     </row>
     <row r="15" spans="13:21">
       <c r="M15">
@@ -4688,6 +5660,15 @@
       <c r="P15">
         <v>450</v>
       </c>
+      <c r="S15">
+        <v>243</v>
+      </c>
+      <c r="T15">
+        <v>0.22490658331731</v>
+      </c>
+      <c r="U15">
+        <v>0.21007282766528701</v>
+      </c>
     </row>
     <row r="16" spans="13:21">
       <c r="M16">
@@ -4702,8 +5683,17 @@
       <c r="P16">
         <v>528</v>
       </c>
-    </row>
-    <row r="17" spans="13:16">
+      <c r="S16">
+        <v>486</v>
+      </c>
+      <c r="T16">
+        <v>0.84780913241129696</v>
+      </c>
+      <c r="U16">
+        <v>0.86894482202294798</v>
+      </c>
+    </row>
+    <row r="17" spans="13:21">
       <c r="M17">
         <v>0.49894734303006599</v>
       </c>
@@ -4716,8 +5706,17 @@
       <c r="P17">
         <v>599</v>
       </c>
-    </row>
-    <row r="18" spans="13:16">
+      <c r="S17">
+        <v>310</v>
+      </c>
+      <c r="T17">
+        <v>0.27102585518594402</v>
+      </c>
+      <c r="U17">
+        <v>0.85877188390634296</v>
+      </c>
+    </row>
+    <row r="18" spans="13:21">
       <c r="M18">
         <v>3.7997552862234198E-2</v>
       </c>
@@ -4730,8 +5729,17 @@
       <c r="P18">
         <v>233</v>
       </c>
-    </row>
-    <row r="19" spans="13:16">
+      <c r="S18">
+        <v>268</v>
+      </c>
+      <c r="T18">
+        <v>0.243228579855159</v>
+      </c>
+      <c r="U18">
+        <v>0.862983925857564</v>
+      </c>
+    </row>
+    <row r="19" spans="13:21">
       <c r="M19">
         <v>0.44123033562478903</v>
       </c>
@@ -4744,8 +5752,17 @@
       <c r="P19">
         <v>455</v>
       </c>
-    </row>
-    <row r="20" spans="13:16">
+      <c r="S19">
+        <v>232</v>
+      </c>
+      <c r="T19">
+        <v>0.13740313187258499</v>
+      </c>
+      <c r="U19">
+        <v>9.0582617622929601E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="13:21">
       <c r="M20">
         <v>0.820620822754073</v>
       </c>
@@ -4758,8 +5775,17 @@
       <c r="P20">
         <v>556</v>
       </c>
-    </row>
-    <row r="21" spans="13:16">
+      <c r="S20">
+        <v>218</v>
+      </c>
+      <c r="T20">
+        <v>0.98953124892358602</v>
+      </c>
+      <c r="U20">
+        <v>0.77071675056441502</v>
+      </c>
+    </row>
+    <row r="21" spans="13:21">
       <c r="M21">
         <v>5.7046083491418903E-2</v>
       </c>
@@ -4772,8 +5798,17 @@
       <c r="P21">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="13:16">
+      <c r="S21">
+        <v>294</v>
+      </c>
+      <c r="T21">
+        <v>0.68350454340665801</v>
+      </c>
+      <c r="U21">
+        <v>0.279667067727149</v>
+      </c>
+    </row>
+    <row r="22" spans="13:21">
       <c r="M22">
         <v>0.67918815670113297</v>
       </c>
@@ -4786,8 +5821,17 @@
       <c r="P22">
         <v>230</v>
       </c>
-    </row>
-    <row r="23" spans="13:16">
+      <c r="S22">
+        <v>195</v>
+      </c>
+      <c r="T22">
+        <v>0.398867870126624</v>
+      </c>
+      <c r="U22">
+        <v>0.526589601027318</v>
+      </c>
+    </row>
+    <row r="23" spans="13:21">
       <c r="M23">
         <v>0.68929942584548698</v>
       </c>
@@ -4800,8 +5844,17 @@
       <c r="P23">
         <v>250</v>
       </c>
-    </row>
-    <row r="24" spans="13:16">
+      <c r="S23">
+        <v>164</v>
+      </c>
+      <c r="T23">
+        <v>0.38652348715295598</v>
+      </c>
+      <c r="U23">
+        <v>0.425462040665956</v>
+      </c>
+    </row>
+    <row r="24" spans="13:21">
       <c r="M24">
         <v>0.81645573391799997</v>
       </c>
@@ -4814,8 +5867,17 @@
       <c r="P24">
         <v>679</v>
       </c>
-    </row>
-    <row r="25" spans="13:16">
+      <c r="S24">
+        <v>273</v>
+      </c>
+      <c r="T24">
+        <v>0.82822236143605299</v>
+      </c>
+      <c r="U24">
+        <v>0.40658455954122702</v>
+      </c>
+    </row>
+    <row r="25" spans="13:21">
       <c r="M25">
         <v>0.245319135320094</v>
       </c>
@@ -4828,8 +5890,17 @@
       <c r="P25">
         <v>230</v>
       </c>
-    </row>
-    <row r="26" spans="13:16">
+      <c r="S25">
+        <v>490</v>
+      </c>
+      <c r="T25">
+        <v>0.57088224604137106</v>
+      </c>
+      <c r="U25">
+        <v>9.4275897145400897E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="13:21">
       <c r="M26">
         <v>0.27739938135521702</v>
       </c>
@@ -4842,8 +5913,17 @@
       <c r="P26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="13:16">
+      <c r="S26">
+        <v>267</v>
+      </c>
+      <c r="T26">
+        <v>0.69837966674477903</v>
+      </c>
+      <c r="U26">
+        <v>0.64395696813103098</v>
+      </c>
+    </row>
+    <row r="27" spans="13:21">
       <c r="M27">
         <v>8.7134915126409307E-2</v>
       </c>
@@ -4856,8 +5936,17 @@
       <c r="P27">
         <v>317</v>
       </c>
-    </row>
-    <row r="28" spans="13:16">
+      <c r="S27">
+        <v>137</v>
+      </c>
+      <c r="T27">
+        <v>0.48455804731306801</v>
+      </c>
+      <c r="U27">
+        <v>0.826316663453037</v>
+      </c>
+    </row>
+    <row r="28" spans="13:21">
       <c r="M28">
         <v>6.7774987787240698E-2</v>
       </c>
@@ -4870,8 +5959,17 @@
       <c r="P28">
         <v>387</v>
       </c>
-    </row>
-    <row r="29" spans="13:16">
+      <c r="S28">
+        <v>158</v>
+      </c>
+      <c r="T28">
+        <v>4.4336767856973699E-2</v>
+      </c>
+      <c r="U28">
+        <v>0.76239043211790003</v>
+      </c>
+    </row>
+    <row r="29" spans="13:21">
       <c r="M29">
         <v>3.91563224567201E-2</v>
       </c>
@@ -4884,8 +5982,17 @@
       <c r="P29">
         <v>230</v>
       </c>
-    </row>
-    <row r="30" spans="13:16">
+      <c r="S29">
+        <v>360</v>
+      </c>
+      <c r="T29">
+        <v>0.27318496317579399</v>
+      </c>
+      <c r="U29">
+        <v>4.2244335694521302E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="13:21">
       <c r="M30">
         <v>0.87010030169353303</v>
       </c>
@@ -4898,8 +6005,17 @@
       <c r="P30">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="13:16">
+      <c r="S30">
+        <v>109</v>
+      </c>
+      <c r="T30">
+        <v>0.496594538190058</v>
+      </c>
+      <c r="U30">
+        <v>0.530613102858702</v>
+      </c>
+    </row>
+    <row r="31" spans="13:21">
       <c r="M31">
         <v>0.83323251028853196</v>
       </c>
@@ -4912,8 +6028,17 @@
       <c r="P31">
         <v>210</v>
       </c>
-    </row>
-    <row r="32" spans="13:16">
+      <c r="S31">
+        <v>99</v>
+      </c>
+      <c r="T31">
+        <v>1.6309743637006401E-2</v>
+      </c>
+      <c r="U31">
+        <v>0.95404846319381598</v>
+      </c>
+    </row>
+    <row r="32" spans="13:21">
       <c r="M32">
         <v>0.68020599487277</v>
       </c>
@@ -4926,8 +6051,17 @@
       <c r="P32">
         <v>230</v>
       </c>
-    </row>
-    <row r="33" spans="13:16">
+      <c r="S32">
+        <v>343</v>
+      </c>
+      <c r="T32">
+        <v>0.26487620694641201</v>
+      </c>
+      <c r="U32">
+        <v>0.147316949878849</v>
+      </c>
+    </row>
+    <row r="33" spans="13:21">
       <c r="M33">
         <v>0.52286271759612002</v>
       </c>
@@ -4940,8 +6074,17 @@
       <c r="P33">
         <v>540</v>
       </c>
-    </row>
-    <row r="34" spans="13:16">
+      <c r="S33">
+        <v>470</v>
+      </c>
+      <c r="T33">
+        <v>0.92254240201264803</v>
+      </c>
+      <c r="U33">
+        <v>0.131359564981958</v>
+      </c>
+    </row>
+    <row r="34" spans="13:21">
       <c r="M34">
         <v>0.43437391514673201</v>
       </c>
@@ -4954,8 +6097,17 @@
       <c r="P34">
         <v>157</v>
       </c>
-    </row>
-    <row r="35" spans="13:16">
+      <c r="S34">
+        <v>201</v>
+      </c>
+      <c r="T34">
+        <v>0.27451934402950701</v>
+      </c>
+      <c r="U34">
+        <v>0.17030128714458301</v>
+      </c>
+    </row>
+    <row r="35" spans="13:21">
       <c r="M35">
         <v>0.412262792685266</v>
       </c>
@@ -4968,8 +6120,17 @@
       <c r="P35">
         <v>344</v>
       </c>
-    </row>
-    <row r="36" spans="13:16">
+      <c r="S35">
+        <v>352</v>
+      </c>
+      <c r="T35">
+        <v>0.17052814277463199</v>
+      </c>
+      <c r="U35">
+        <v>0.87226315272445898</v>
+      </c>
+    </row>
+    <row r="36" spans="13:21">
       <c r="M36">
         <v>0.120870326703281</v>
       </c>
@@ -4982,8 +6143,17 @@
       <c r="P36">
         <v>230</v>
       </c>
-    </row>
-    <row r="37" spans="13:16">
+      <c r="S36">
+        <v>318</v>
+      </c>
+      <c r="T36">
+        <v>0.31225336204906801</v>
+      </c>
+      <c r="U36">
+        <v>0.96000903983284003</v>
+      </c>
+    </row>
+    <row r="37" spans="13:21">
       <c r="M37">
         <v>0.63613821456739394</v>
       </c>
@@ -4996,8 +6166,17 @@
       <c r="P37">
         <v>570</v>
       </c>
-    </row>
-    <row r="38" spans="13:16">
+      <c r="S37">
+        <v>105</v>
+      </c>
+      <c r="T37">
+        <v>0.118424292774472</v>
+      </c>
+      <c r="U37">
+        <v>0.60321193137080897</v>
+      </c>
+    </row>
+    <row r="38" spans="13:21">
       <c r="M38">
         <v>0.72852810969122195</v>
       </c>
@@ -5010,8 +6189,17 @@
       <c r="P38">
         <v>341</v>
       </c>
-    </row>
-    <row r="39" spans="13:16">
+      <c r="S38">
+        <v>183</v>
+      </c>
+      <c r="T38">
+        <v>0.61317251978456699</v>
+      </c>
+      <c r="U38">
+        <v>0.66816314164776103</v>
+      </c>
+    </row>
+    <row r="39" spans="13:21">
       <c r="M39">
         <v>1.61053094301211E-2</v>
       </c>
@@ -5024,8 +6212,17 @@
       <c r="P39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="13:16">
+      <c r="S39">
+        <v>189</v>
+      </c>
+      <c r="T39">
+        <v>0.93835032639007399</v>
+      </c>
+      <c r="U39">
+        <v>6.2867979474326194E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="13:21">
       <c r="M40">
         <v>0.81703897928243197</v>
       </c>
@@ -5038,8 +6235,17 @@
       <c r="P40">
         <v>410</v>
       </c>
-    </row>
-    <row r="41" spans="13:16">
+      <c r="S40">
+        <v>275</v>
+      </c>
+      <c r="T40">
+        <v>0.70137774021640598</v>
+      </c>
+      <c r="U40">
+        <v>0.24861513934801099</v>
+      </c>
+    </row>
+    <row r="41" spans="13:21">
       <c r="M41">
         <v>0.86893739671147197</v>
       </c>
@@ -5052,8 +6258,17 @@
       <c r="P41">
         <v>370</v>
       </c>
-    </row>
-    <row r="42" spans="13:16">
+      <c r="S41">
+        <v>327</v>
+      </c>
+      <c r="T41">
+        <v>0.96603780599074396</v>
+      </c>
+      <c r="U41">
+        <v>0.293694941582472</v>
+      </c>
+    </row>
+    <row r="42" spans="13:21">
       <c r="M42">
         <v>0.61901713552426596</v>
       </c>
@@ -5066,8 +6281,17 @@
       <c r="P42">
         <v>68</v>
       </c>
-    </row>
-    <row r="43" spans="13:16">
+      <c r="S42">
+        <v>401</v>
+      </c>
+      <c r="T42">
+        <v>0.595390948695112</v>
+      </c>
+      <c r="U42">
+        <v>7.3933005873462299E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="13:21">
       <c r="M43">
         <v>0.44705268551362098</v>
       </c>
@@ -5080,8 +6304,17 @@
       <c r="P43">
         <v>163</v>
       </c>
-    </row>
-    <row r="44" spans="13:16">
+      <c r="S43">
+        <v>274</v>
+      </c>
+      <c r="T43">
+        <v>0.27301448358124802</v>
+      </c>
+      <c r="U43">
+        <v>0.61872701870307201</v>
+      </c>
+    </row>
+    <row r="44" spans="13:21">
       <c r="M44">
         <v>0.195711184834545</v>
       </c>
@@ -5094,8 +6327,17 @@
       <c r="P44">
         <v>520</v>
       </c>
-    </row>
-    <row r="45" spans="13:16">
+      <c r="S44">
+        <v>111</v>
+      </c>
+      <c r="T44">
+        <v>0.33408283497233199</v>
+      </c>
+      <c r="U44">
+        <v>0.91356460409895901</v>
+      </c>
+    </row>
+    <row r="45" spans="13:21">
       <c r="M45">
         <v>0.59180785320402995</v>
       </c>
@@ -5108,8 +6350,17 @@
       <c r="P45">
         <v>146</v>
       </c>
-    </row>
-    <row r="46" spans="13:16">
+      <c r="S45">
+        <v>198</v>
+      </c>
+      <c r="T45">
+        <v>0.87100759890594304</v>
+      </c>
+      <c r="U45">
+        <v>0.44709530618632798</v>
+      </c>
+    </row>
+    <row r="46" spans="13:21">
       <c r="M46">
         <v>0.17503819558474901</v>
       </c>
@@ -5122,8 +6373,17 @@
       <c r="P46">
         <v>469</v>
       </c>
-    </row>
-    <row r="47" spans="13:16">
+      <c r="S46">
+        <v>253</v>
+      </c>
+      <c r="T46">
+        <v>0.247307847351352</v>
+      </c>
+      <c r="U46">
+        <v>0.55588414101239603</v>
+      </c>
+    </row>
+    <row r="47" spans="13:21">
       <c r="M47">
         <v>0.45095608962774802</v>
       </c>
@@ -5136,8 +6396,17 @@
       <c r="P47">
         <v>20</v>
       </c>
-    </row>
-    <row r="48" spans="13:16">
+      <c r="S47">
+        <v>199</v>
+      </c>
+      <c r="T47">
+        <v>0.68305595362589</v>
+      </c>
+      <c r="U47">
+        <v>0.47213502698917797</v>
+      </c>
+    </row>
+    <row r="48" spans="13:21">
       <c r="M48">
         <v>0.73614833565391602</v>
       </c>
@@ -5150,8 +6419,17 @@
       <c r="P48">
         <v>427</v>
       </c>
-    </row>
-    <row r="49" spans="13:16">
+      <c r="S48">
+        <v>313</v>
+      </c>
+      <c r="T48">
+        <v>0.68720461028088797</v>
+      </c>
+      <c r="U48">
+        <v>0.70186904731414701</v>
+      </c>
+    </row>
+    <row r="49" spans="13:21">
       <c r="M49">
         <v>0.120590102949423</v>
       </c>
@@ -5164,8 +6442,17 @@
       <c r="P49">
         <v>307</v>
       </c>
-    </row>
-    <row r="50" spans="13:16">
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>5.5698255847577399E-2</v>
+      </c>
+      <c r="U49">
+        <v>0.75546275083093295</v>
+      </c>
+    </row>
+    <row r="50" spans="13:21">
       <c r="M50">
         <v>0.994048501388476</v>
       </c>
@@ -5178,8 +6465,17 @@
       <c r="P50">
         <v>352</v>
       </c>
-    </row>
-    <row r="51" spans="13:16">
+      <c r="S50">
+        <v>260</v>
+      </c>
+      <c r="T50">
+        <v>0.17427143868721801</v>
+      </c>
+      <c r="U50">
+        <v>0.48875905034848899</v>
+      </c>
+    </row>
+    <row r="51" spans="13:21">
       <c r="M51">
         <v>0.140787785385</v>
       </c>
@@ -5192,8 +6488,17 @@
       <c r="P51">
         <v>344</v>
       </c>
-    </row>
-    <row r="52" spans="13:16">
+      <c r="S51">
+        <v>147</v>
+      </c>
+      <c r="T51">
+        <v>0.244354087953711</v>
+      </c>
+      <c r="U51">
+        <v>0.56228167495669101</v>
+      </c>
+    </row>
+    <row r="52" spans="13:21">
       <c r="M52">
         <v>0.45156592011208302</v>
       </c>
@@ -5206,8 +6511,17 @@
       <c r="P52">
         <v>420</v>
       </c>
-    </row>
-    <row r="53" spans="13:16">
+      <c r="S52">
+        <v>137</v>
+      </c>
+      <c r="T52">
+        <v>0.48898543659951399</v>
+      </c>
+      <c r="U52">
+        <v>5.4630775763472098E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="13:21">
       <c r="M53">
         <v>8.2364802299602996E-2</v>
       </c>
@@ -5220,8 +6534,17 @@
       <c r="P53">
         <v>309</v>
       </c>
-    </row>
-    <row r="54" spans="13:16">
+      <c r="S53">
+        <v>241</v>
+      </c>
+      <c r="T53">
+        <v>0.294797196686158</v>
+      </c>
+      <c r="U53">
+        <v>0.927183414621778</v>
+      </c>
+    </row>
+    <row r="54" spans="13:21">
       <c r="M54">
         <v>0.85868773660707098</v>
       </c>
@@ -5233,6 +6556,15 @@
       </c>
       <c r="P54">
         <v>100</v>
+      </c>
+      <c r="S54">
+        <v>174</v>
+      </c>
+      <c r="T54">
+        <v>0.58146880838336501</v>
+      </c>
+      <c r="U54">
+        <v>0.810088336564732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final final data and graphs
</commit_message>
<xml_diff>
--- a/Summary Analysis.xlsx
+++ b/Summary Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="28460" windowHeight="17280" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1960" yWindow="0" windowWidth="26160" windowHeight="16920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="time spent" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
   <si>
     <t>x axis</t>
   </si>
@@ -58,9 +58,6 @@
     <t>average time spent in that activity (out of 1440)</t>
   </si>
   <si>
-    <t>DATA REQUIRED</t>
-  </si>
-  <si>
     <t>Total time spent</t>
   </si>
   <si>
@@ -76,76 +73,10 @@
     <t>Read</t>
   </si>
   <si>
-    <t>Student 1</t>
-  </si>
-  <si>
-    <t>Student 2</t>
-  </si>
-  <si>
-    <t>Student 3</t>
-  </si>
-  <si>
-    <t>Student 4</t>
-  </si>
-  <si>
-    <t>Student 5</t>
-  </si>
-  <si>
-    <t>Student 6</t>
-  </si>
-  <si>
-    <t>Student 7</t>
-  </si>
-  <si>
-    <t>Student 8</t>
-  </si>
-  <si>
-    <t>Student 9</t>
-  </si>
-  <si>
-    <t>Student 10</t>
-  </si>
-  <si>
-    <t>Student 11</t>
-  </si>
-  <si>
-    <t>Student 12</t>
-  </si>
-  <si>
-    <t>Student 13</t>
-  </si>
-  <si>
-    <t>Student 14</t>
-  </si>
-  <si>
-    <t>Student 15</t>
-  </si>
-  <si>
-    <t>Student 16</t>
-  </si>
-  <si>
-    <t>Student 17</t>
-  </si>
-  <si>
-    <t>Student 18</t>
-  </si>
-  <si>
-    <t>Student 19</t>
-  </si>
-  <si>
-    <t>Student 20</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
     <t>SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lazy? </t>
-  </si>
-  <si>
-    <t>Count of each activity</t>
   </si>
   <si>
     <t>A</t>
@@ -264,6 +195,51 @@
   <si>
     <t>learnChance</t>
   </si>
+  <si>
+    <t>summarized data</t>
+  </si>
+  <si>
+    <t>average over 20 runs</t>
+  </si>
+  <si>
+    <t>lazy</t>
+  </si>
+  <si>
+    <t>indifferent</t>
+  </si>
+  <si>
+    <t>friendly</t>
+  </si>
+  <si>
+    <t>bookworm</t>
+  </si>
+  <si>
+    <t>hardworking</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>lazy?</t>
+  </si>
+  <si>
+    <t>going</t>
+  </si>
+  <si>
+    <t>solo</t>
+  </si>
+  <si>
+    <t>spoink</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Spoink</t>
+  </si>
+  <si>
+    <t>Solo   Spoink</t>
+  </si>
 </sst>
 </file>
 
@@ -328,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -351,8 +327,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,8 +396,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -410,8 +426,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -435,6 +456,16 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -458,6 +489,16 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -472,10 +513,845 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFD2F7"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>% time spent in each activity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'time spent'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="50000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="350000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'time spent'!$F$4:$G$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>going</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>spoink</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>indifferent</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>friendly</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>bookworm</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>indifferent</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>friendly</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>bookworm</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>solo</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v> </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'time spent'!$H$4:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>596.1550000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>660.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>595.6299999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512.4200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>557.8199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>505.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>759.9724999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'time spent'!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Consult</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:tint val="100000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:tint val="50000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="350000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'time spent'!$F$4:$G$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>going</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>spoink</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>indifferent</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>friendly</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>bookworm</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>indifferent</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>friendly</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>bookworm</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>solo</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v> </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'time spent'!$I$4:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>261.8000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140.2475</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>308.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>451.1599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>353.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>464.6650000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>114.4275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'time spent'!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Collaborate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:tint val="100000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:tint val="50000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="350000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'time spent'!$F$4:$G$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>going</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>spoink</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>indifferent</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>friendly</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>bookworm</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>indifferent</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>friendly</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>bookworm</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>solo</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v> </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'time spent'!$J$4:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>420.2049999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>548.8725000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>195.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300.315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>379.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>208.175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>262.085</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1175.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'time spent'!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Read</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="100000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="50000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="350000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'time spent'!$F$4:$G$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>lazy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>hardworking</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>going</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>spoink</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>indifferent</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>friendly</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>bookworm</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>indifferent</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>friendly</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>bookworm</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>solo</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v> </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'time spent'!$K$4:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>200.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117.745</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>385.3525000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>229.775</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>195.2175</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>316.8124999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>438.1524999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>165.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="2114366504"/>
+        <c:axId val="2117533048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2114366504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2117533048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2117533048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2114366504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0713851839948578"/>
+          <c:y val="0.0623501199040767"/>
+          <c:w val="0.928614816005142"/>
+          <c:h val="0.840064200608018"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'time spent'!$L$4:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>270.7775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>143.1475</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>348.0124999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>449.3325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>353.2075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>483.785</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>767.19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2108447160"/>
+        <c:axId val="2111630616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2108447160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2111630616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2111630616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2108447160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -522,16 +1398,35 @@
             <c:v>Lazy</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'2a knowledge by pref'!$E$8:$E$10</c:f>
+                <c:f>'2a knowledge by pref'!$E$8:$E$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
                     <c:v>73.12</c:v>
                   </c:pt>
@@ -541,23 +1436,29 @@
                   <c:pt idx="2">
                     <c:v>53.8</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23.0</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'2a knowledge by pref'!$E$11:$E$13</c:f>
+                <c:f>'2a knowledge by pref'!$E$8:$E$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>60.2</c:v>
+                    <c:v>73.12</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>40.8</c:v>
+                    <c:v>47.62</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>69.8</c:v>
+                    <c:v>53.8</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -565,9 +1466,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'2a knowledge by pref'!$C$8:$C$10</c:f>
+              <c:f>'2a knowledge by pref'!$C$8:$C$11</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Indecisive</c:v>
                 </c:pt>
@@ -576,16 +1477,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Bookworm</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Solo   Spoink</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2a knowledge by pref'!$D$8:$D$10</c:f>
+              <c:f>'2a knowledge by pref'!$D$8:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>274.02</c:v>
                 </c:pt>
@@ -594,6 +1498,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>352.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -606,16 +1513,55 @@
             <c:v>Hardworking</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="62000">
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="65000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="95000">
+                    <a:srgbClr val="FFD2F7"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'2a knowledge by pref'!$E$11:$E$13</c:f>
+                <c:f>'2a knowledge by pref'!$E$12:$E$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
                     <c:v>60.2</c:v>
                   </c:pt>
@@ -625,15 +1571,18 @@
                   <c:pt idx="2">
                     <c:v>69.8</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>112.4</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'2a knowledge by pref'!$E$11:$E$13</c:f>
+                <c:f>'2a knowledge by pref'!$E$12:$E$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
                     <c:v>60.2</c:v>
                   </c:pt>
@@ -643,15 +1592,18 @@
                   <c:pt idx="2">
                     <c:v>69.8</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>112.4</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'2a knowledge by pref'!$C$8:$C$10</c:f>
+              <c:f>'2a knowledge by pref'!$C$8:$C$11</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Indecisive</c:v>
                 </c:pt>
@@ -660,16 +1612,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Bookworm</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Solo   Spoink</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2a knowledge by pref'!$D$11:$D$13</c:f>
+              <c:f>'2a knowledge by pref'!$D$12:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>448.0</c:v>
                 </c:pt>
@@ -678,6 +1633,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>480.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>767.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,11 +1650,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2074995864"/>
-        <c:axId val="2075002424"/>
+        <c:axId val="2111877880"/>
+        <c:axId val="2111807608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2074995864"/>
+        <c:axId val="2111877880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,7 +1683,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075002424"/>
+        <c:crossAx val="2111807608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -733,7 +1691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2075002424"/>
+        <c:axId val="2111807608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -744,7 +1702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074995864"/>
+        <c:crossAx val="2111877880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -766,7 +1724,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -796,7 +1754,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1055,11 +2012,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2075042536"/>
-        <c:axId val="2075047992"/>
+        <c:axId val="2111515832"/>
+        <c:axId val="2114497304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2075042536"/>
+        <c:axId val="2111515832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,14 +2038,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075047992"/>
+        <c:crossAx val="2114497304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1096,7 +2052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2075047992"/>
+        <c:axId val="2114497304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200.0"/>
@@ -1107,14 +2063,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075042536"/>
+        <c:crossAx val="2111515832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1149,7 +2104,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1164,7 +2119,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1189,7 +2143,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1529,7 +2482,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1861,30 +2813,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075104392"/>
-        <c:axId val="2075109432"/>
+        <c:axId val="2114596904"/>
+        <c:axId val="2111014328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075104392"/>
+        <c:axId val="2114596904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075109432"/>
+        <c:crossAx val="2111014328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075109432"/>
+        <c:axId val="2111014328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1893,21 +2844,19 @@
         <c:majorGridlines/>
         <c:minorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075104392"/>
+        <c:crossAx val="2114596904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1922,7 +2871,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1937,7 +2886,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2674,51 +3622,48 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2074206648"/>
-        <c:axId val="2074201640"/>
+        <c:axId val="2099363176"/>
+        <c:axId val="2099368264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2074206648"/>
+        <c:axId val="2099363176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074201640"/>
+        <c:crossAx val="2099368264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2074201640"/>
+        <c:axId val="2099368264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074206648"/>
+        <c:crossAx val="2099363176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2733,7 +3678,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2763,7 +3708,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4026,7 +4970,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4034,51 +4977,48 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095195256"/>
-        <c:axId val="2090322264"/>
+        <c:axId val="2116553336"/>
+        <c:axId val="2116558360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095195256"/>
+        <c:axId val="2116553336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090322264"/>
+        <c:crossAx val="2116558360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2090322264"/>
+        <c:axId val="2116558360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095195256"/>
+        <c:crossAx val="2116553336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4093,7 +5033,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4128,7 +5068,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5398,51 +6337,48 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2104814184"/>
-        <c:axId val="2104726184"/>
+        <c:axId val="2115389960"/>
+        <c:axId val="2115384984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2104814184"/>
+        <c:axId val="2115389960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104726184"/>
+        <c:crossAx val="2115384984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2104726184"/>
+        <c:axId val="2115384984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104814184"/>
+        <c:crossAx val="2115389960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5461,16 +6397,130 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>596899</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>69851</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190498</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="5" name="Group 4"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4889499" y="2736851"/>
+          <a:ext cx="7848599" cy="4006850"/>
+          <a:chOff x="4889500" y="2546350"/>
+          <a:chExt cx="6959600" cy="3651250"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="2" name="Chart 1"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="4889500" y="2546350"/>
+          <a:ext cx="6959600" cy="3651250"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Chart 2"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="4900762" y="2569909"/>
+          <a:ext cx="5979850" cy="3416300"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="TextBox 3"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10858500" y="3441700"/>
+            <a:ext cx="982010" cy="261610"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>---</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Knowledge</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5492,7 +6542,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5527,7 +6577,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5592,7 +6642,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5658,8 +6708,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:G13" totalsRowShown="0">
-  <autoFilter ref="A7:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:G15" totalsRowShown="0">
+  <autoFilter ref="A7:G15"/>
   <tableColumns count="7">
     <tableColumn id="1" name="NumA"/>
     <tableColumn id="6" name="Prefs"/>
@@ -6013,10 +7063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6025,100 +7075,127 @@
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="F2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="F4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="1">
+        <v>596.15500000000009</v>
+      </c>
+      <c r="I4" s="1">
+        <v>261.80000000000007</v>
+      </c>
+      <c r="J4" s="1">
+        <v>420.20499999999993</v>
+      </c>
+      <c r="K4" s="1">
+        <v>200.05</v>
+      </c>
+      <c r="L4" s="8">
+        <v>270.77749999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="F5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="1">
+        <v>660.21</v>
+      </c>
+      <c r="I5" s="1">
+        <v>140.2475</v>
+      </c>
+      <c r="J5" s="1">
+        <v>548.87250000000006</v>
+      </c>
+      <c r="K5" s="1">
+        <v>117.74499999999998</v>
+      </c>
+      <c r="L5" s="8">
+        <v>143.14749999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="F6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="1">
+        <v>595.62999999999988</v>
+      </c>
+      <c r="I6" s="1">
+        <v>308.34000000000003</v>
+      </c>
+      <c r="J6" s="1">
+        <v>195.45</v>
+      </c>
+      <c r="K6" s="1">
+        <v>385.35250000000008</v>
+      </c>
+      <c r="L6" s="8">
+        <v>348.01249999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -6129,17 +7206,28 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:16">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="1">
+        <v>512.42000000000007</v>
+      </c>
+      <c r="I7" s="1">
+        <v>451.15999999999985</v>
+      </c>
+      <c r="J7" s="1">
+        <v>300.315</v>
+      </c>
+      <c r="K7" s="1">
+        <v>229.77500000000001</v>
+      </c>
+      <c r="L7" s="8">
+        <v>449.33249999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -6150,241 +7238,125 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="1">
+        <v>557.81999999999994</v>
+      </c>
+      <c r="I8" s="1">
+        <v>353.21000000000004</v>
+      </c>
+      <c r="J8" s="1">
+        <v>379.54999999999995</v>
+      </c>
+      <c r="K8" s="1">
+        <v>195.21750000000003</v>
+      </c>
+      <c r="L8" s="8">
+        <v>353.20749999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="1">
+        <v>505.89</v>
+      </c>
+      <c r="I9" s="1">
+        <v>464.66500000000008</v>
+      </c>
+      <c r="J9" s="1">
+        <v>208.17500000000001</v>
+      </c>
+      <c r="K9" s="1">
+        <v>316.81249999999994</v>
+      </c>
+      <c r="L9" s="9">
+        <v>483.78500000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="1">
+        <v>759.97249999999974</v>
+      </c>
+      <c r="I10" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="J10" s="1">
+        <v>262.08499999999998</v>
+      </c>
+      <c r="K10" s="1">
+        <v>438.15249999999986</v>
+      </c>
+      <c r="L10" s="9">
+        <v>33.14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:16">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10">
+        <v>114.42750000000001</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1175.1199999999999</v>
+      </c>
+      <c r="K11" s="10">
+        <v>165.65</v>
+      </c>
+      <c r="L11" s="11">
+        <v>767.18999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="F13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="F16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="6:11">
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="6:11">
-      <c r="F18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="6:11">
-      <c r="F19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="6:11">
-      <c r="F20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="6:11">
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="6:11">
-      <c r="F22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="6:11">
-      <c r="F23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="25" spans="6:11">
-      <c r="F25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" t="e">
-        <f>AVERAGE(H4:H23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" t="e">
-        <f t="shared" ref="I25:K25" si="0">AVERAGE(I4:I23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J25" t="e">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <f>AVERAGE(H4:H10)</f>
+        <v>598.29964285714266</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:L12" si="0">AVERAGE(I4:I10)</f>
+        <v>282.77464285714285</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K25" t="e">
+        <v>330.66464285714289</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="6:11">
-      <c r="F26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" t="e">
-        <f>STDEV(H4:H23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" t="e">
-        <f t="shared" ref="I26:K26" si="1">STDEV(I4:I23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J26" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K26" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>269.01499999999999</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>297.34321428571423</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6397,8 +7369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6416,7 +7388,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -6424,7 +7396,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -6449,54 +7421,54 @@
     </row>
     <row r="4" spans="1:20">
       <c r="H4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="N4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="O4" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="Q4" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="R4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="S4" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="T4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -6581,25 +7553,25 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -6649,7 +7621,7 @@
         <v>6222</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>274.02</v>
@@ -6712,7 +7684,7 @@
         <v>6141</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>140.6</v>
@@ -6775,7 +7747,7 @@
         <v>6114</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>352</v>
@@ -6831,28 +7803,26 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>20</v>
       </c>
-      <c r="B11">
-        <v>3333</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11">
-        <v>448</v>
-      </c>
-      <c r="E11">
+      <c r="B11" s="4">
+        <v>4044</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="9">
+        <v>33.14</v>
+      </c>
+      <c r="E11" s="12">
         <f>2*Table1[[#This Row],[SD group Knowledge]]</f>
-        <v>60.2</v>
-      </c>
-      <c r="F11">
-        <v>30.1</v>
-      </c>
-      <c r="G11">
-        <v>188.2</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F11" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="G11" s="4"/>
       <c r="H11">
         <v>7</v>
       </c>
@@ -6898,23 +7868,23 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>3252</v>
+        <v>3333</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D12">
-        <v>353.1</v>
+        <v>448</v>
       </c>
       <c r="E12">
         <f>2*Table1[[#This Row],[SD group Knowledge]]</f>
-        <v>40.799999999999997</v>
+        <v>60.2</v>
       </c>
       <c r="F12">
-        <v>20.399999999999999</v>
+        <v>30.1</v>
       </c>
       <c r="G12">
-        <v>151.69999999999999</v>
+        <v>188.2</v>
       </c>
       <c r="H12">
         <v>8</v>
@@ -6961,23 +7931,23 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>3225</v>
+        <v>3252</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D13">
-        <v>480.2</v>
+        <v>353.1</v>
       </c>
       <c r="E13">
         <f>2*Table1[[#This Row],[SD group Knowledge]]</f>
-        <v>69.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="F13">
-        <v>34.9</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="G13">
-        <v>186.4</v>
+        <v>151.69999999999999</v>
       </c>
       <c r="H13">
         <v>9</v>
@@ -7020,6 +7990,28 @@
       </c>
     </row>
     <row r="14" spans="1:20">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>3225</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>480.2</v>
+      </c>
+      <c r="E14">
+        <f>2*Table1[[#This Row],[SD group Knowledge]]</f>
+        <v>69.8</v>
+      </c>
+      <c r="F14">
+        <v>34.9</v>
+      </c>
+      <c r="G14">
+        <v>186.4</v>
+      </c>
       <c r="H14">
         <v>10</v>
       </c>
@@ -7061,6 +8053,26 @@
       </c>
     </row>
     <row r="15" spans="1:20">
+      <c r="A15" s="4">
+        <v>20</v>
+      </c>
+      <c r="B15" s="4">
+        <v>444</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="11">
+        <v>767.18999999999994</v>
+      </c>
+      <c r="E15" s="12">
+        <f>2*Table1[[#This Row],[SD group Knowledge]]</f>
+        <v>112.4</v>
+      </c>
+      <c r="F15" s="4">
+        <v>56.2</v>
+      </c>
+      <c r="G15" s="4"/>
       <c r="H15">
         <v>11</v>
       </c>
@@ -7102,6 +8114,7 @@
       </c>
     </row>
     <row r="16" spans="1:20">
+      <c r="E16" s="3"/>
       <c r="H16">
         <v>12</v>
       </c>
@@ -7142,7 +8155,8 @@
         <v>171.98255725508901</v>
       </c>
     </row>
-    <row r="17" spans="8:20">
+    <row r="17" spans="5:20">
+      <c r="E17" s="3"/>
       <c r="H17">
         <v>13</v>
       </c>
@@ -7183,7 +8197,7 @@
         <v>188.267894235846</v>
       </c>
     </row>
-    <row r="18" spans="8:20">
+    <row r="18" spans="5:20">
       <c r="H18">
         <v>14</v>
       </c>
@@ -7224,7 +8238,7 @@
         <v>152.31320743091999</v>
       </c>
     </row>
-    <row r="19" spans="8:20">
+    <row r="19" spans="5:20">
       <c r="H19">
         <v>15</v>
       </c>
@@ -7265,7 +8279,7 @@
         <v>169.16478263577901</v>
       </c>
     </row>
-    <row r="20" spans="8:20">
+    <row r="20" spans="5:20">
       <c r="H20">
         <v>16</v>
       </c>
@@ -7306,7 +8320,7 @@
         <v>176.29922978008901</v>
       </c>
     </row>
-    <row r="21" spans="8:20">
+    <row r="21" spans="5:20">
       <c r="H21">
         <v>17</v>
       </c>
@@ -7347,7 +8361,7 @@
         <v>166.63003457075899</v>
       </c>
     </row>
-    <row r="22" spans="8:20">
+    <row r="22" spans="5:20">
       <c r="H22">
         <v>18</v>
       </c>
@@ -7388,7 +8402,7 @@
         <v>216.218280302203</v>
       </c>
     </row>
-    <row r="23" spans="8:20">
+    <row r="23" spans="5:20">
       <c r="H23">
         <v>19</v>
       </c>
@@ -7429,7 +8443,7 @@
         <v>242.020198156661</v>
       </c>
     </row>
-    <row r="24" spans="8:20">
+    <row r="24" spans="5:20">
       <c r="H24">
         <v>20</v>
       </c>
@@ -7470,9 +8484,9 @@
         <v>180.92489718403201</v>
       </c>
     </row>
-    <row r="26" spans="8:20">
+    <row r="26" spans="5:20">
       <c r="H26" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="I26">
         <f xml:space="preserve"> AVERAGE(I5:I24)</f>
@@ -7483,49 +8497,49 @@
         <v>143.60200000000003</v>
       </c>
       <c r="K26">
-        <f t="shared" ref="K26" si="0" xml:space="preserve"> AVERAGE(K5:K24)</f>
+        <f xml:space="preserve"> AVERAGE(K5:K24)</f>
         <v>140.5925</v>
       </c>
       <c r="L26">
-        <f t="shared" ref="L26" si="1">AVERAGE(L5:L24)</f>
+        <f>AVERAGE(L5:L24)</f>
         <v>107.24624096649136</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26" si="2" xml:space="preserve"> AVERAGE(M5:M24)</f>
+        <f xml:space="preserve"> AVERAGE(M5:M24)</f>
         <v>352.005</v>
       </c>
       <c r="N26">
-        <f t="shared" ref="N26" si="3">AVERAGE(N5:N24)</f>
+        <f>AVERAGE(N5:N24)</f>
         <v>153.89061519652003</v>
       </c>
       <c r="O26">
-        <f t="shared" ref="O26" si="4" xml:space="preserve"> AVERAGE(O5:O24)</f>
+        <f xml:space="preserve"> AVERAGE(O5:O24)</f>
         <v>447.99999999999989</v>
       </c>
       <c r="P26">
-        <f t="shared" ref="P26" si="5">AVERAGE(P5:P24)</f>
+        <f>AVERAGE(P5:P24)</f>
         <v>188.15908367509741</v>
       </c>
       <c r="Q26">
-        <f t="shared" ref="Q26" si="6" xml:space="preserve"> AVERAGE(Q5:Q24)</f>
+        <f xml:space="preserve"> AVERAGE(Q5:Q24)</f>
         <v>353.09500000000003</v>
       </c>
       <c r="R26">
-        <f t="shared" ref="R26" si="7">AVERAGE(R5:R24)</f>
+        <f>AVERAGE(R5:R24)</f>
         <v>151.68645101499999</v>
       </c>
       <c r="S26">
-        <f t="shared" ref="S26" si="8" xml:space="preserve"> AVERAGE(S5:S24)</f>
+        <f xml:space="preserve"> AVERAGE(S5:S24)</f>
         <v>480.24749999999995</v>
       </c>
       <c r="T26">
-        <f t="shared" ref="T26" si="9">AVERAGE(T5:T24)</f>
+        <f>AVERAGE(T5:T24)</f>
         <v>186.42218834578506</v>
       </c>
     </row>
-    <row r="27" spans="8:20">
+    <row r="27" spans="5:20">
       <c r="H27" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="I27">
         <f>STDEV(I5:I24)</f>
@@ -7552,9 +8566,9 @@
         <v>34.880431818180945</v>
       </c>
     </row>
-    <row r="28" spans="8:20">
+    <row r="28" spans="5:20">
       <c r="H28" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="I28">
         <f>I27/SQRT(20)</f>
@@ -7581,9 +8595,9 @@
         <v>7.7995016629999174</v>
       </c>
     </row>
-    <row r="29" spans="8:20">
+    <row r="29" spans="5:20">
       <c r="H29" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="I29">
         <f>2*I28</f>
@@ -7648,7 +8662,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -7656,57 +8670,57 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="I3" s="7" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="H4" s="7" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="H5" s="7">
         <v>1</v>
@@ -7755,19 +8769,19 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="H7" s="7">
         <v>3</v>
@@ -8091,7 +9105,7 @@
         <v>363.77499999999998</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="I16">
         <f xml:space="preserve"> AVERAGE(I5:I14)</f>
@@ -8121,7 +9135,7 @@
     <row r="17" spans="4:13">
       <c r="D17" s="3"/>
       <c r="H17" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="I17">
         <f>STDEV(I5:I14)</f>
@@ -8138,7 +9152,7 @@
     </row>
     <row r="18" spans="4:13">
       <c r="H18" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="I18">
         <f>I17/SQRT(20)</f>
@@ -8155,7 +9169,7 @@
     </row>
     <row r="19" spans="4:13">
       <c r="H19" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="I19">
         <f>2*I18</f>
@@ -8197,10 +9211,10 @@
   <sheetData>
     <row r="1" spans="13:21">
       <c r="M1" s="7" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="U1" s="7"/>
     </row>
@@ -8214,33 +9228,33 @@
     </row>
     <row r="3" spans="13:21">
       <c r="M3" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="O3" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="13:21">
       <c r="M4" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="P4" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="S4" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="T4" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="U4" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="13:21">
@@ -9409,24 +10423,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>